<commit_message>
Supplied some important required data
</commit_message>
<xml_diff>
--- a/testdata/sample2-1.xlsx
+++ b/testdata/sample2-1.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="115">
   <si>
     <t>Title</t>
   </si>
@@ -316,19 +316,43 @@
     <t>Event X</t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Espionage</t>
+  </si>
+  <si>
+    <t>Imprisonments</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>San Francisco, California, United States of America</t>
+  </si>
+  <si>
     <t>Bordeaux</t>
   </si>
   <si>
     <t>False Imprisonment</t>
   </si>
   <si>
+    <t>Female</t>
+  </si>
+  <si>
     <t>Journalist</t>
   </si>
   <si>
+    <t>Male</t>
+  </si>
+  <si>
     <t>The Tor Project</t>
   </si>
   <si>
     <t>Software Developer</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
   <si>
     <t>American Military</t>
@@ -1879,7 +1903,7 @@
   <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1964,29 +1988,59 @@
       <c r="A2" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
+      <c r="B2" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="42" t="n">
+        <v>41733</v>
+      </c>
+      <c r="F2" s="42" t="n">
+        <v>41800</v>
+      </c>
+      <c r="G2" s="42" t="n">
+        <v>41735</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="J2" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="L2" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="M2" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="N2" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="O2" s="41" t="s">
+        <v>100</v>
+      </c>
       <c r="P2" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="Q2" s="41"/>
+      <c r="Q2" s="41" t="s">
+        <v>101</v>
+      </c>
       <c r="R2" s="43" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="S2" s="44" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2038,17 +2092,23 @@
         <v>31</v>
       </c>
       <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
+      <c r="E4" s="22" t="n">
+        <v>30663</v>
+      </c>
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
+      <c r="H4" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>100</v>
+      </c>
       <c r="J4" s="21"/>
       <c r="K4" s="23" t="s">
         <v>93</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="N4" s="16"/>
       <c r="O4" s="16"/>
@@ -2064,17 +2124,23 @@
         <v>32</v>
       </c>
       <c r="D5" s="21"/>
-      <c r="E5" s="22"/>
+      <c r="E5" s="22" t="n">
+        <v>27847</v>
+      </c>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
+      <c r="H5" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>100</v>
+      </c>
       <c r="J5" s="21"/>
       <c r="K5" s="23" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="L5" s="23" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="N5" s="16"/>
       <c r="O5" s="16"/>
@@ -2090,14 +2156,20 @@
         <v>33</v>
       </c>
       <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
+      <c r="E6" s="22" t="n">
+        <v>18963</v>
+      </c>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
+      <c r="H6" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>109</v>
+      </c>
       <c r="J6" s="21"/>
       <c r="K6" s="24" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="L6" s="24" t="s">
         <v>47</v>
@@ -2148,12 +2220,12 @@
       <c r="A8" s="40"/>
       <c r="B8" s="26"/>
       <c r="C8" s="24" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
       <c r="F8" s="21" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
@@ -2173,12 +2245,12 @@
       <c r="A9" s="40"/>
       <c r="B9" s="26"/>
       <c r="C9" s="24" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
@@ -2272,7 +2344,7 @@
       <c r="B13" s="28"/>
       <c r="C13" s="21"/>
       <c r="D13" s="24" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>

</xml_diff>

<commit_message>
Filled out the rest of the fields to fix parsing
</commit_message>
<xml_diff>
--- a/testdata/sample2-1.xlsx
+++ b/testdata/sample2-1.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="135">
   <si>
     <t>Title</t>
   </si>
@@ -142,6 +142,15 @@
     <t>Witness</t>
   </si>
   <si>
+    <t>Eliza</t>
+  </si>
+  <si>
+    <t>111-123-4321</t>
+  </si>
+  <si>
+    <t>Montreal, QC, Canada</t>
+  </si>
+  <si>
     <t>Female</t>
   </si>
   <si>
@@ -154,6 +163,12 @@
     <t>Victim</t>
   </si>
   <si>
+    <t>Gary</t>
+  </si>
+  <si>
+    <t>111-555-1234</t>
+  </si>
+  <si>
     <t>Male</t>
   </si>
   <si>
@@ -166,6 +181,15 @@
     <t>Perpetrator</t>
   </si>
   <si>
+    <t>Hank</t>
+  </si>
+  <si>
+    <t>111-123-1234</t>
+  </si>
+  <si>
+    <t>Washington, United States of America</t>
+  </si>
+  <si>
     <t>no</t>
   </si>
   <si>
@@ -199,19 +223,55 @@
     <t>John Green</t>
   </si>
   <si>
+    <t>Complaint 1</t>
+  </si>
+  <si>
+    <t>Response 1</t>
+  </si>
+  <si>
     <t>United Nations</t>
   </si>
   <si>
+    <t>Complaint 2</t>
+  </si>
+  <si>
+    <t>Response 2</t>
+  </si>
+  <si>
     <t>Hanna Flemming</t>
   </si>
   <si>
+    <t>Complaint 3</t>
+  </si>
+  <si>
+    <t>Response 3</t>
+  </si>
+  <si>
     <t>Amnesty International</t>
   </si>
   <si>
+    <t>Complaint 4</t>
+  </si>
+  <si>
+    <t>Response 4</t>
+  </si>
+  <si>
     <t>Source</t>
   </si>
   <si>
+    <t>Ada Lovelace</t>
+  </si>
+  <si>
+    <t>Charles Babbage</t>
+  </si>
+  <si>
+    <t>Alan Turing</t>
+  </si>
+  <si>
     <t>Report</t>
+  </si>
+  <si>
+    <t>Text text text</t>
   </si>
   <si>
     <t>Professions</t>
@@ -750,7 +810,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -893,8 +953,8 @@
   </sheetPr>
   <dimension ref="1:15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1091,24 +1151,32 @@
       <c r="C4" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="21"/>
+      <c r="D4" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="E4" s="22" t="n">
         <v>30663</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
+      <c r="F4" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>41</v>
+      </c>
       <c r="H4" s="21" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="21"/>
+      <c r="J4" s="21" t="s">
+        <v>20</v>
+      </c>
       <c r="K4" s="23" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="N4" s="16"/>
       <c r="O4" s="16"/>
@@ -1121,26 +1189,34 @@
       <c r="A5" s="7"/>
       <c r="B5" s="19"/>
       <c r="C5" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="21"/>
+        <v>45</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>46</v>
+      </c>
       <c r="E5" s="22" t="n">
         <v>27847</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
+      <c r="F5" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>41</v>
+      </c>
       <c r="H5" s="21" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="I5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="21"/>
+      <c r="J5" s="21" t="s">
+        <v>20</v>
+      </c>
       <c r="K5" s="23" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="L5" s="23" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="N5" s="16"/>
       <c r="O5" s="16"/>
@@ -1153,26 +1229,34 @@
       <c r="A6" s="7"/>
       <c r="B6" s="19"/>
       <c r="C6" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="21"/>
+        <v>51</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>52</v>
+      </c>
       <c r="E6" s="22" t="n">
         <v>18963</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
+      <c r="F6" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="H6" s="21" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" s="21"/>
+        <v>55</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>20</v>
+      </c>
       <c r="K6" s="24" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
@@ -1184,25 +1268,25 @@
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="14" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="I7" s="25"/>
       <c r="J7" s="16"/>
@@ -1220,15 +1304,23 @@
       <c r="A8" s="7"/>
       <c r="B8" s="26"/>
       <c r="C8" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
+        <v>65</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>67</v>
+      </c>
       <c r="F8" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+        <v>68</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="I8" s="25"/>
       <c r="J8" s="16"/>
       <c r="K8" s="16"/>
@@ -1245,15 +1337,23 @@
       <c r="A9" s="7"/>
       <c r="B9" s="26"/>
       <c r="C9" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+        <v>71</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>73</v>
+      </c>
       <c r="F9" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+        <v>74</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>76</v>
+      </c>
       <c r="I9" s="25"/>
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
@@ -1269,7 +1369,7 @@
     <row r="10" customFormat="false" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
       <c r="B10" s="27" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>29</v>
@@ -1296,9 +1396,11 @@
     <row r="11" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="7"/>
       <c r="B11" s="28"/>
-      <c r="C11" s="21"/>
+      <c r="C11" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="D11" s="24" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
@@ -1319,9 +1421,11 @@
     <row r="12" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="7"/>
       <c r="B12" s="28"/>
-      <c r="C12" s="21"/>
+      <c r="C12" s="21" t="s">
+        <v>79</v>
+      </c>
       <c r="D12" s="24" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
@@ -1342,9 +1446,11 @@
     <row r="13" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="7"/>
       <c r="B13" s="28"/>
-      <c r="C13" s="21"/>
+      <c r="C13" s="21" t="s">
+        <v>80</v>
+      </c>
       <c r="D13" s="24" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
@@ -1365,7 +1471,7 @@
     <row r="14" customFormat="false" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="7"/>
       <c r="B14" s="27" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C14" s="29"/>
       <c r="D14" s="29"/>
@@ -1387,7 +1493,9 @@
     </row>
     <row r="15" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="7"/>
-      <c r="B15" s="30"/>
+      <c r="B15" s="30" t="s">
+        <v>82</v>
+      </c>
       <c r="C15" s="29"/>
       <c r="D15" s="29"/>
       <c r="E15" s="29"/>
@@ -1447,7 +1555,7 @@
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>29</v>
@@ -1456,25 +1564,25 @@
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19"/>
       <c r="B3" s="34" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19"/>
       <c r="B4" s="34" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19"/>
       <c r="B5" s="34" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19"/>
       <c r="B6" s="34" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1517,10 +1625,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="33" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="C1" s="33" t="s">
         <v>1</v>
@@ -1529,19 +1637,19 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19"/>
       <c r="B2" s="34" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19"/>
       <c r="B3" s="34" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1578,10 +1686,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="33" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="C1" s="33" t="s">
         <v>1</v>
@@ -1590,19 +1698,19 @@
     <row r="2" customFormat="false" ht="25.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19"/>
       <c r="B2" s="34" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19"/>
       <c r="B3" s="34" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1638,172 +1746,172 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="35" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="36" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="36" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="36" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="36" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="36" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="36" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="36" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="36" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="36" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="36" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="36" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="36" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="36" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="36" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="36" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="36" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="36" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="36" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="36" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="36" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="36" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="36" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="36" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="36" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="36" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="36" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="36" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="36" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="36" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="36" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="36" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="36" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="36" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1886,13 +1994,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2030,7 +2138,7 @@
     </row>
     <row r="2" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="40" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>20</v>
@@ -2142,17 +2250,17 @@
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
       <c r="H4" s="21" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>23</v>
       </c>
       <c r="J4" s="21"/>
       <c r="K4" s="23" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="N4" s="16"/>
       <c r="O4" s="16"/>
@@ -2165,7 +2273,7 @@
       <c r="A5" s="40"/>
       <c r="B5" s="19"/>
       <c r="C5" s="20" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="22" t="n">
@@ -2174,17 +2282,17 @@
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
       <c r="H5" s="21" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="I5" s="21" t="s">
         <v>23</v>
       </c>
       <c r="J5" s="21"/>
       <c r="K5" s="23" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="L5" s="23" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="N5" s="16"/>
       <c r="O5" s="16"/>
@@ -2197,7 +2305,7 @@
       <c r="A6" s="40"/>
       <c r="B6" s="19"/>
       <c r="C6" s="20" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="22" t="n">
@@ -2206,17 +2314,17 @@
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
       <c r="H6" s="21" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="J6" s="21"/>
       <c r="K6" s="24" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
@@ -2228,25 +2336,25 @@
     <row r="7" customFormat="false" ht="25.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="40"/>
       <c r="B7" s="14" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="I7" s="25"/>
       <c r="J7" s="42"/>
@@ -2264,12 +2372,12 @@
       <c r="A8" s="40"/>
       <c r="B8" s="26"/>
       <c r="C8" s="24" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
       <c r="F8" s="21" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
@@ -2289,12 +2397,12 @@
       <c r="A9" s="40"/>
       <c r="B9" s="26"/>
       <c r="C9" s="24" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
@@ -2313,7 +2421,7 @@
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="40"/>
       <c r="B10" s="27" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>29</v>
@@ -2342,7 +2450,7 @@
       <c r="B11" s="28"/>
       <c r="C11" s="21"/>
       <c r="D11" s="24" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
@@ -2365,7 +2473,7 @@
       <c r="B12" s="28"/>
       <c r="C12" s="21"/>
       <c r="D12" s="24" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
@@ -2388,7 +2496,7 @@
       <c r="B13" s="28"/>
       <c r="C13" s="21"/>
       <c r="D13" s="24" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
@@ -2409,7 +2517,7 @@
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="40"/>
       <c r="B14" s="27" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="43"/>

</xml_diff>

<commit_message>
Removed actions from template
</commit_message>
<xml_diff>
--- a/testdata/sample2-1.xlsx
+++ b/testdata/sample2-1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="117">
   <si>
     <t>Title</t>
   </si>
@@ -199,235 +199,181 @@
     <t>Military</t>
   </si>
   <si>
-    <t>Actions</t>
-  </si>
-  <si>
-    <t>State authorities approached</t>
-  </si>
-  <si>
-    <t>Complaint to state authority</t>
-  </si>
-  <si>
-    <t>Response from state authority</t>
-  </si>
-  <si>
-    <t>International authorities approached</t>
-  </si>
-  <si>
-    <t>Complaint to international authority</t>
-  </si>
-  <si>
-    <t>Response from international authority</t>
-  </si>
-  <si>
-    <t>John Green</t>
-  </si>
-  <si>
-    <t>Complaint 1</t>
-  </si>
-  <si>
-    <t>Response 1</t>
-  </si>
-  <si>
-    <t>United Nations</t>
-  </si>
-  <si>
-    <t>Complaint 2</t>
-  </si>
-  <si>
-    <t>Response 2</t>
-  </si>
-  <si>
-    <t>Hanna Flemming</t>
-  </si>
-  <si>
-    <t>Complaint 3</t>
-  </si>
-  <si>
-    <t>Response 3</t>
-  </si>
-  <si>
-    <t>Amnesty International</t>
-  </si>
-  <si>
-    <t>Complaint 4</t>
-  </si>
-  <si>
-    <t>Response 4</t>
+    <t>Sources</t>
+  </si>
+  <si>
+    <t>Ada Lovelace</t>
+  </si>
+  <si>
+    <t>Charles Babbage</t>
+  </si>
+  <si>
+    <t>Alan Turing</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Text text text</t>
+  </si>
+  <si>
+    <t>Professions</t>
+  </si>
+  <si>
+    <t>Jounalist</t>
+  </si>
+  <si>
+    <t>Software developer</t>
+  </si>
+  <si>
+    <t>Politician</t>
+  </si>
+  <si>
+    <t>International Authorities</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>UN</t>
+  </si>
+  <si>
+    <t>President of the U.S.A. for two terms</t>
+  </si>
+  <si>
+    <t>ICC</t>
+  </si>
+  <si>
+    <t>Prime Minister of Canada</t>
+  </si>
+  <si>
+    <t>State Authority</t>
+  </si>
+  <si>
+    <t>Revolutionariy committee</t>
+  </si>
+  <si>
+    <t>Pretty much everywhere</t>
+  </si>
+  <si>
+    <t>Castros office</t>
+  </si>
+  <si>
+    <t>Behind the tobacco shop</t>
+  </si>
+  <si>
+    <t>International Standard</t>
+  </si>
+  <si>
+    <t>Right to self determination</t>
+  </si>
+  <si>
+    <t>Right to exploit natural  wealth &amp; resources</t>
+  </si>
+  <si>
+    <t>State duty to protect, promote &amp; fulfil human rights</t>
+  </si>
+  <si>
+    <t>Non Discrimination/Equality</t>
+  </si>
+  <si>
+    <t>Right to Life</t>
+  </si>
+  <si>
+    <t>Prohibition of Torture or CIDT</t>
+  </si>
+  <si>
+    <t>Prohibition Against Slavery, Servitude &amp; Forced Labour/Child Labour</t>
+  </si>
+  <si>
+    <t>Right to Liberty and Security of the Person</t>
+  </si>
+  <si>
+    <t>Equality before the law</t>
+  </si>
+  <si>
+    <t>Protection of the Law/Due Process</t>
+  </si>
+  <si>
+    <t>Protection from imprisonment for Debt</t>
+  </si>
+  <si>
+    <t>Freedom  of Movement/Residence</t>
+  </si>
+  <si>
+    <t>Right to Privacy</t>
+  </si>
+  <si>
+    <t>Freedom of thought/conscience/religion</t>
+  </si>
+  <si>
+    <t>Freedom of expression</t>
+  </si>
+  <si>
+    <t>protection from hate Speech</t>
+  </si>
+  <si>
+    <t>Freedom of Association &amp; Assembly</t>
+  </si>
+  <si>
+    <t>Right to Dignity &amp; Intergrity</t>
+  </si>
+  <si>
+    <t>Right to marry and found a family</t>
+  </si>
+  <si>
+    <t>Right of Child to name, identity and nationality</t>
+  </si>
+  <si>
+    <t>Right to political participation</t>
+  </si>
+  <si>
+    <t>Right to culture, religion, language and protection against harmful practices</t>
+  </si>
+  <si>
+    <t>Right to Work/decent working conditions/unionise/collective bargaining</t>
+  </si>
+  <si>
+    <t>Right to Social Security</t>
+  </si>
+  <si>
+    <t>Right to adequate standard of living – food, shelter, clothing</t>
+  </si>
+  <si>
+    <t>Right to the Highest Attainable Standard of mental &amp; physical health</t>
+  </si>
+  <si>
+    <t>Right to education</t>
+  </si>
+  <si>
+    <t>Protection of Women</t>
+  </si>
+  <si>
+    <t>Protection of Children</t>
+  </si>
+  <si>
+    <t>Protection of Minorities (sexual orientation/migrants/disabled etc)</t>
+  </si>
+  <si>
+    <t>War crimes</t>
+  </si>
+  <si>
+    <t>Genocide &amp; Ethnic Cleansing</t>
+  </si>
+  <si>
+    <t>Enforced disappearance</t>
+  </si>
+  <si>
+    <t>Digital solutions for civil society</t>
+  </si>
+  <si>
+    <t>5605 de Gaspe, suite 204, Montreal, QC, Canada</t>
+  </si>
+  <si>
+    <t>Event X</t>
   </si>
   <si>
     <t>Source</t>
-  </si>
-  <si>
-    <t>Ada Lovelace</t>
-  </si>
-  <si>
-    <t>Charles Babbage</t>
-  </si>
-  <si>
-    <t>Alan Turing</t>
-  </si>
-  <si>
-    <t>Report</t>
-  </si>
-  <si>
-    <t>Text text text</t>
-  </si>
-  <si>
-    <t>Professions</t>
-  </si>
-  <si>
-    <t>Jounalist</t>
-  </si>
-  <si>
-    <t>Software developer</t>
-  </si>
-  <si>
-    <t>Politician</t>
-  </si>
-  <si>
-    <t>International Authorities</t>
-  </si>
-  <si>
-    <t>Body</t>
-  </si>
-  <si>
-    <t>UN</t>
-  </si>
-  <si>
-    <t>President of the U.S.A. for two terms</t>
-  </si>
-  <si>
-    <t>ICC</t>
-  </si>
-  <si>
-    <t>Prime Minister of Canada</t>
-  </si>
-  <si>
-    <t>State Authority</t>
-  </si>
-  <si>
-    <t>Revolutionariy committee</t>
-  </si>
-  <si>
-    <t>Pretty much everywhere</t>
-  </si>
-  <si>
-    <t>Castros office</t>
-  </si>
-  <si>
-    <t>Behind the tobacco shop</t>
-  </si>
-  <si>
-    <t>International Standard</t>
-  </si>
-  <si>
-    <t>Right to self determination</t>
-  </si>
-  <si>
-    <t>Right to exploit natural  wealth &amp; resources</t>
-  </si>
-  <si>
-    <t>State duty to protect, promote &amp; fulfil human rights</t>
-  </si>
-  <si>
-    <t>Non Discrimination/Equality</t>
-  </si>
-  <si>
-    <t>Right to Life</t>
-  </si>
-  <si>
-    <t>Prohibition of Torture or CIDT</t>
-  </si>
-  <si>
-    <t>Prohibition Against Slavery, Servitude &amp; Forced Labour/Child Labour</t>
-  </si>
-  <si>
-    <t>Right to Liberty and Security of the Person</t>
-  </si>
-  <si>
-    <t>Equality before the law</t>
-  </si>
-  <si>
-    <t>Protection of the Law/Due Process</t>
-  </si>
-  <si>
-    <t>Protection from imprisonment for Debt</t>
-  </si>
-  <si>
-    <t>Freedom  of Movement/Residence</t>
-  </si>
-  <si>
-    <t>Right to Privacy</t>
-  </si>
-  <si>
-    <t>Freedom of thought/conscience/religion</t>
-  </si>
-  <si>
-    <t>Freedom of expression</t>
-  </si>
-  <si>
-    <t>protection from hate Speech</t>
-  </si>
-  <si>
-    <t>Freedom of Association &amp; Assembly</t>
-  </si>
-  <si>
-    <t>Right to Dignity &amp; Intergrity</t>
-  </si>
-  <si>
-    <t>Right to marry and found a family</t>
-  </si>
-  <si>
-    <t>Right of Child to name, identity and nationality</t>
-  </si>
-  <si>
-    <t>Right to political participation</t>
-  </si>
-  <si>
-    <t>Right to culture, religion, language and protection against harmful practices</t>
-  </si>
-  <si>
-    <t>Right to Work/decent working conditions/unionise/collective bargaining</t>
-  </si>
-  <si>
-    <t>Right to Social Security</t>
-  </si>
-  <si>
-    <t>Right to adequate standard of living – food, shelter, clothing</t>
-  </si>
-  <si>
-    <t>Right to the Highest Attainable Standard of mental &amp; physical health</t>
-  </si>
-  <si>
-    <t>Right to education</t>
-  </si>
-  <si>
-    <t>Protection of Women</t>
-  </si>
-  <si>
-    <t>Protection of Children</t>
-  </si>
-  <si>
-    <t>Protection of Minorities (sexual orientation/migrants/disabled etc)</t>
-  </si>
-  <si>
-    <t>War crimes</t>
-  </si>
-  <si>
-    <t>Genocide &amp; Ethnic Cleansing</t>
-  </si>
-  <si>
-    <t>Enforced disappearance</t>
-  </si>
-  <si>
-    <t>Digital solutions for civil society</t>
-  </si>
-  <si>
-    <t>5605 de Gaspe, suite 204, Montreal, QC, Canada</t>
-  </si>
-  <si>
-    <t>Event X</t>
   </si>
 </sst>
 </file>
@@ -689,7 +635,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -787,14 +733,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -951,10 +889,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:15"/>
+  <dimension ref="1:12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1103,7 +1041,7 @@
       <c r="T2" s="12"/>
       <c r="U2" s="13"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7"/>
       <c r="B3" s="14" t="s">
         <v>27</v>
@@ -1265,30 +1203,22 @@
       <c r="R6" s="17"/>
       <c r="S6" s="18"/>
     </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="25" t="s">
         <v>58</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="I7" s="25"/>
+        <v>36</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
       <c r="L7" s="16"/>
@@ -1303,25 +1233,17 @@
     <row r="8" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
       <c r="B8" s="26"/>
-      <c r="C8" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="I8" s="25"/>
+      <c r="C8" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
       <c r="J8" s="16"/>
       <c r="K8" s="16"/>
       <c r="L8" s="16"/>
@@ -1336,25 +1258,17 @@
     <row r="9" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7"/>
       <c r="B9" s="26"/>
-      <c r="C9" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="I9" s="25"/>
+      <c r="C9" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
       <c r="L9" s="16"/>
@@ -1366,16 +1280,14 @@
       <c r="R9" s="17"/>
       <c r="S9" s="18"/>
     </row>
-    <row r="10" customFormat="false" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
-      <c r="B10" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>36</v>
+      <c r="B10" s="26"/>
+      <c r="C10" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>49</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
@@ -1393,20 +1305,18 @@
       <c r="R10" s="17"/>
       <c r="S10" s="18"/>
     </row>
-    <row r="11" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="7"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
+      <c r="B11" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
       <c r="L11" s="16"/>
@@ -1418,109 +1328,34 @@
       <c r="R11" s="17"/>
       <c r="S11" s="18"/>
     </row>
-    <row r="12" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="7"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
+      <c r="B12" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
       <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="18"/>
-    </row>
-    <row r="13" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="18"/>
-    </row>
-    <row r="14" customFormat="false" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7"/>
-      <c r="B14" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="18"/>
-    </row>
-    <row r="15" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7"/>
-      <c r="B15" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="31"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="31"/>
-      <c r="S15" s="32"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A2:A15"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:M15"/>
-    <mergeCell ref="E10:I13"/>
-    <mergeCell ref="C14:I15"/>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="E7:I10"/>
+    <mergeCell ref="C11:I12"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1554,34 +1389,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="33" t="s">
+      <c r="A2" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="31" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19"/>
-      <c r="B3" s="34" t="s">
-        <v>84</v>
+      <c r="B3" s="32" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19"/>
-      <c r="B4" s="34" t="s">
-        <v>85</v>
+      <c r="B4" s="32" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19"/>
-      <c r="B5" s="34" t="s">
-        <v>86</v>
+      <c r="B5" s="32" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19"/>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="32" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1624,32 +1459,32 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" s="33" t="s">
+      <c r="A1" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19"/>
-      <c r="B2" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>90</v>
+      <c r="B2" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19"/>
-      <c r="B3" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="34" t="s">
-        <v>92</v>
+      <c r="B3" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1685,32 +1520,32 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" s="33" t="s">
+      <c r="A1" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="25.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19"/>
-      <c r="B2" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>95</v>
+      <c r="B2" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19"/>
-      <c r="B3" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="34" t="s">
-        <v>97</v>
+      <c r="B3" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1745,173 +1580,173 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="34" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="34" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="34" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="34" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="34" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="36" t="s">
+    <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="34" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="36" t="s">
+    <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="34" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="36" t="s">
+    <row r="23" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="34" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="36" t="s">
+    <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="34" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="36" t="s">
+    <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="34" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="36" t="s">
+    <row r="26" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="34" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="36" t="s">
+    <row r="27" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="34" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="36" t="s">
+    <row r="28" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="34" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="36" t="s">
+    <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="34" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="36" t="s">
+    <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="34" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="36" t="s">
+    <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="34" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="36" t="s">
+    <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="34" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="36" t="s">
+    <row r="33" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="34" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="36" t="s">
+    <row r="34" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="34" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="36" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="36" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="36" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="36" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="36" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="36" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="36" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="36" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="36" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="36" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="36" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="36" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="36" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="36" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="36" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="36" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="36" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="36" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="36" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1944,10 +1779,10 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="35" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1982,13 +1817,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="36" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1997,10 +1832,10 @@
         <v>43</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2032,7 +1867,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2052,10 +1887,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V15"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2132,13 +1967,13 @@
       <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
     </row>
     <row r="2" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="40" t="s">
-        <v>134</v>
+      <c r="A2" s="38" t="s">
+        <v>115</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>20</v>
@@ -2195,8 +2030,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="40"/>
+    <row r="3" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="38"/>
       <c r="B3" s="14" t="s">
         <v>27</v>
       </c>
@@ -2235,10 +2070,10 @@
       <c r="P3" s="17"/>
       <c r="Q3" s="16"/>
       <c r="R3" s="17"/>
-      <c r="S3" s="41"/>
+      <c r="S3" s="39"/>
     </row>
     <row r="4" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="40"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="19"/>
       <c r="C4" s="20" t="s">
         <v>38</v>
@@ -2267,10 +2102,10 @@
       <c r="P4" s="17"/>
       <c r="Q4" s="16"/>
       <c r="R4" s="17"/>
-      <c r="S4" s="41"/>
+      <c r="S4" s="39"/>
     </row>
     <row r="5" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="40"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="19"/>
       <c r="C5" s="20" t="s">
         <v>45</v>
@@ -2299,10 +2134,10 @@
       <c r="P5" s="17"/>
       <c r="Q5" s="16"/>
       <c r="R5" s="17"/>
-      <c r="S5" s="41"/>
+      <c r="S5" s="39"/>
     </row>
     <row r="6" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="40"/>
+      <c r="A6" s="38"/>
       <c r="B6" s="19"/>
       <c r="C6" s="20" t="s">
         <v>51</v>
@@ -2331,240 +2166,153 @@
       <c r="P6" s="17"/>
       <c r="Q6" s="16"/>
       <c r="R6" s="17"/>
-      <c r="S6" s="41"/>
-    </row>
-    <row r="7" customFormat="false" ht="25.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="40"/>
-      <c r="B7" s="14" t="s">
-        <v>58</v>
+      <c r="S6" s="39"/>
+    </row>
+    <row r="7" customFormat="false" ht="18.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="38"/>
+      <c r="B7" s="25" t="s">
+        <v>116</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="I7" s="25"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
+        <v>36</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
       <c r="N7" s="16"/>
       <c r="O7" s="16"/>
       <c r="P7" s="17"/>
       <c r="Q7" s="16"/>
       <c r="R7" s="17"/>
-      <c r="S7" s="41"/>
+      <c r="S7" s="39"/>
     </row>
     <row r="8" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="40"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="26"/>
-      <c r="C8" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
       <c r="N8" s="16"/>
       <c r="O8" s="16"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="16"/>
       <c r="R8" s="17"/>
-      <c r="S8" s="41"/>
+      <c r="S8" s="39"/>
     </row>
     <row r="9" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="40"/>
+      <c r="A9" s="38"/>
       <c r="B9" s="26"/>
-      <c r="C9" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="42"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
       <c r="N9" s="16"/>
       <c r="O9" s="16"/>
       <c r="P9" s="17"/>
       <c r="Q9" s="16"/>
       <c r="R9" s="17"/>
-      <c r="S9" s="41"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="40"/>
-      <c r="B10" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>36</v>
+      <c r="S9" s="39"/>
+    </row>
+    <row r="10" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="38"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="24" t="s">
+        <v>49</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
       <c r="I10" s="16"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="16"/>
       <c r="R10" s="17"/>
-      <c r="S10" s="41"/>
-    </row>
-    <row r="11" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="40"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
+      <c r="S10" s="39"/>
+    </row>
+    <row r="11" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="38"/>
+      <c r="B11" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
       <c r="N11" s="16"/>
       <c r="O11" s="16"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="16"/>
       <c r="R11" s="17"/>
-      <c r="S11" s="41"/>
-    </row>
-    <row r="12" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="40"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="41"/>
-    </row>
-    <row r="13" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="40"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="41"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="40"/>
-      <c r="B14" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="41"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="40"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="42"/>
-      <c r="N15" s="42"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="44"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="44"/>
-      <c r="S15" s="45"/>
+      <c r="S11" s="39"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="38"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="42"/>
+      <c r="Q12" s="40"/>
+      <c r="R12" s="42"/>
+      <c r="S12" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A2:A15"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:M15"/>
-    <mergeCell ref="E10:I13"/>
-    <mergeCell ref="C14:I15"/>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="E7:I10"/>
+    <mergeCell ref="C11:I12"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added report text in cell next to header
</commit_message>
<xml_diff>
--- a/testdata/sample2-1.xlsx
+++ b/testdata/sample2-1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" state="visible" r:id="rId2"/>
@@ -214,7 +214,7 @@
     <t>Report</t>
   </si>
   <si>
-    <t>Text text text</t>
+    <t>Text Text Text Text Text Text Text Text Text Text </t>
   </si>
   <si>
     <t>Professions</t>
@@ -384,7 +384,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="MMMM\ D&quot;, &quot;YYYY"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -441,6 +441,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -744,11 +750,11 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -768,11 +774,11 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -780,7 +786,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -891,8 +897,8 @@
   </sheetPr>
   <dimension ref="1:12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -978,6 +984,12 @@
       </c>
       <c r="T1" s="4"/>
       <c r="U1" s="5"/>
+      <c r="AMD1" s="0"/>
+      <c r="AME1" s="0"/>
+      <c r="AMF1" s="0"/>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1310,7 +1322,9 @@
       <c r="B11" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="C11" s="27" t="s">
+        <v>63</v>
+      </c>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
@@ -1330,9 +1344,7 @@
     </row>
     <row r="12" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="7"/>
-      <c r="B12" s="28" t="s">
-        <v>63</v>
-      </c>
+      <c r="B12" s="28"/>
       <c r="C12" s="27"/>
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
@@ -1889,8 +1901,8 @@
   </sheetPr>
   <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>